<commit_message>
update fig3 for new split date
</commit_message>
<xml_diff>
--- a/outcome/appendix/Figure Data/Fig.6 data.xlsx
+++ b/outcome/appendix/Figure Data/Fig.6 data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="278">
   <si>
     <t xml:space="preserve">class</t>
   </si>
@@ -857,15 +857,6 @@
   <si>
     <t xml:space="preserve">X2023.01.01</t>
   </si>
-  <si>
-    <t xml:space="preserve">X2023.02.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X2023.03.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X2023.04.01</t>
-  </si>
 </sst>
 </file>
 
@@ -2082,15 +2073,6 @@
       <c r="AM1" t="s">
         <v>277</v>
       </c>
-      <c r="AN1" t="s">
-        <v>278</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>279</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>280</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -2210,15 +2192,6 @@
       <c r="AM2" t="n">
         <v>0.263230303201223</v>
       </c>
-      <c r="AN2" t="n">
-        <v>0.413387626727509</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>0.230047498307442</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>0.122341422050048</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -2338,15 +2311,6 @@
       <c r="AM3" t="n">
         <v>0.153869376301927</v>
       </c>
-      <c r="AN3" t="n">
-        <v>0.428186865746061</v>
-      </c>
-      <c r="AO3" t="n">
-        <v>0.253411428865701</v>
-      </c>
-      <c r="AP3" t="n">
-        <v>0.213641068813313</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -2466,15 +2430,6 @@
       <c r="AM4" t="n">
         <v>0.665809427808503</v>
       </c>
-      <c r="AN4" t="n">
-        <v>0.987588742858819</v>
-      </c>
-      <c r="AO4" t="n">
-        <v>0.756918061292538</v>
-      </c>
-      <c r="AP4" t="n">
-        <v>0.810319629505895</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -2594,15 +2549,6 @@
       <c r="AM5" t="n">
         <v>-3.42464009737254</v>
       </c>
-      <c r="AN5" t="n">
-        <v>-3.39940055405</v>
-      </c>
-      <c r="AO5" t="n">
-        <v>-3.4947337506017</v>
-      </c>
-      <c r="AP5" t="n">
-        <v>-3.2856518195182</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -2722,15 +2668,6 @@
       <c r="AM6" t="n">
         <v>0.595432590846561</v>
       </c>
-      <c r="AN6" t="n">
-        <v>0.463270577579243</v>
-      </c>
-      <c r="AO6" t="n">
-        <v>0.365339489339483</v>
-      </c>
-      <c r="AP6" t="n">
-        <v>0.329230260915579</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -2850,15 +2787,6 @@
       <c r="AM7" t="n">
         <v>0.667649722621047</v>
       </c>
-      <c r="AN7" t="n">
-        <v>1.12899305989526</v>
-      </c>
-      <c r="AO7" t="n">
-        <v>0.560191901814442</v>
-      </c>
-      <c r="AP7" t="n">
-        <v>0.838479780897082</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -2978,15 +2906,6 @@
       <c r="AM8" t="n">
         <v>-0.0705474489869138</v>
       </c>
-      <c r="AN8" t="n">
-        <v>-0.143488438138486</v>
-      </c>
-      <c r="AO8" t="n">
-        <v>0.175109359749559</v>
-      </c>
-      <c r="AP8" t="n">
-        <v>0.259525600607175</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -3106,15 +3025,6 @@
       <c r="AM9" t="n">
         <v>0.376515468677237</v>
       </c>
-      <c r="AN9" t="n">
-        <v>0.440093363621778</v>
-      </c>
-      <c r="AO9" t="n">
-        <v>0.418062409358431</v>
-      </c>
-      <c r="AP9" t="n">
-        <v>0.416972281161938</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -3234,15 +3144,6 @@
       <c r="AM10" t="n">
         <v>0.324539836178846</v>
       </c>
-      <c r="AN10" t="n">
-        <v>0.354409543587638</v>
-      </c>
-      <c r="AO10" t="n">
-        <v>0.476448402857847</v>
-      </c>
-      <c r="AP10" t="n">
-        <v>0.434326926549304</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -3362,15 +3263,6 @@
       <c r="AM11" t="n">
         <v>0.535547041180719</v>
       </c>
-      <c r="AN11" t="n">
-        <v>0.578880457447692</v>
-      </c>
-      <c r="AO11" t="n">
-        <v>0.499770134961523</v>
-      </c>
-      <c r="AP11" t="n">
-        <v>0.507315066533857</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -3490,15 +3382,6 @@
       <c r="AM12" t="n">
         <v>0.406207073412492</v>
       </c>
-      <c r="AN12" t="n">
-        <v>0.519703250957127</v>
-      </c>
-      <c r="AO12" t="n">
-        <v>0.376455002322061</v>
-      </c>
-      <c r="AP12" t="n">
-        <v>0.392807811997798</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -3618,15 +3501,6 @@
       <c r="AM13" t="n">
         <v>0.355989261606786</v>
       </c>
-      <c r="AN13" t="n">
-        <v>0.471734051545736</v>
-      </c>
-      <c r="AO13" t="n">
-        <v>0.501710969402215</v>
-      </c>
-      <c r="AP13" t="n">
-        <v>0.580083403017813</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -3746,15 +3620,6 @@
       <c r="AM14" t="n">
         <v>-1.27447414535202</v>
       </c>
-      <c r="AN14" t="n">
-        <v>-1.28867082553521</v>
-      </c>
-      <c r="AO14" t="n">
-        <v>-0.88827469804023</v>
-      </c>
-      <c r="AP14" t="n">
-        <v>-0.948318550492076</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -3874,15 +3739,6 @@
       <c r="AM15" t="n">
         <v>-0.223546525250862</v>
       </c>
-      <c r="AN15" t="n">
-        <v>-0.428289481945481</v>
-      </c>
-      <c r="AO15" t="n">
-        <v>-0.137332879471191</v>
-      </c>
-      <c r="AP15" t="n">
-        <v>-0.108871346271135</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -4002,15 +3858,6 @@
       <c r="AM16" t="n">
         <v>-0.00259513083178143</v>
       </c>
-      <c r="AN16" t="n">
-        <v>0.232422845330032</v>
-      </c>
-      <c r="AO16" t="n">
-        <v>0.462568110113179</v>
-      </c>
-      <c r="AP16" t="n">
-        <v>0.504881523977443</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
@@ -4130,15 +3977,6 @@
       <c r="AM17" t="n">
         <v>1.72778649746387</v>
       </c>
-      <c r="AN17" t="n">
-        <v>1.00448805227021</v>
-      </c>
-      <c r="AO17" t="n">
-        <v>1.46144691989213</v>
-      </c>
-      <c r="AP17" t="n">
-        <v>0.987487759212215</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -4258,15 +4096,6 @@
       <c r="AM18" t="n">
         <v>0.47460609290998</v>
       </c>
-      <c r="AN18" t="n">
-        <v>0.0432909745533368</v>
-      </c>
-      <c r="AO18" t="n">
-        <v>0.305383771525753</v>
-      </c>
-      <c r="AP18" t="n">
-        <v>0.478522679470589</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -4386,15 +4215,6 @@
       <c r="AM19" t="n">
         <v>-0.617194144022358</v>
       </c>
-      <c r="AN19" t="n">
-        <v>-0.441485112092623</v>
-      </c>
-      <c r="AO19" t="n">
-        <v>-0.215952056008671</v>
-      </c>
-      <c r="AP19" t="n">
-        <v>-0.425345030924153</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -4514,15 +4334,6 @@
       <c r="AM20" t="n">
         <v>-0.0127085434799633</v>
       </c>
-      <c r="AN20" t="n">
-        <v>-0.912815189455095</v>
-      </c>
-      <c r="AO20" t="n">
-        <v>-0.929794630762767</v>
-      </c>
-      <c r="AP20" t="n">
-        <v>-0.695806559425522</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -4642,15 +4453,6 @@
       <c r="AM21" t="n">
         <v>-0.909778505929621</v>
       </c>
-      <c r="AN21" t="n">
-        <v>-1.05113704457584</v>
-      </c>
-      <c r="AO21" t="n">
-        <v>-1.54651252586074</v>
-      </c>
-      <c r="AP21" t="n">
-        <v>-1.99467874840897</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
@@ -4770,15 +4572,6 @@
       <c r="AM22" t="n">
         <v>-1.49268743353787</v>
       </c>
-      <c r="AN22" t="n">
-        <v>-1.14992629800796</v>
-      </c>
-      <c r="AO22" t="n">
-        <v>-1.09692410616963</v>
-      </c>
-      <c r="AP22" t="n">
-        <v>-1.13210673842294</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -4898,15 +4691,6 @@
       <c r="AM23" t="n">
         <v>0.358292119639118</v>
       </c>
-      <c r="AN23" t="n">
-        <v>0.363187223794476</v>
-      </c>
-      <c r="AO23" t="n">
-        <v>0.308171412091469</v>
-      </c>
-      <c r="AP23" t="n">
-        <v>0.332118020429082</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
@@ -5026,15 +4810,6 @@
       <c r="AM24" t="n">
         <v>0.671811264828821</v>
       </c>
-      <c r="AN24" t="n">
-        <v>0.665487971094159</v>
-      </c>
-      <c r="AO24" t="n">
-        <v>0.419909780054107</v>
-      </c>
-      <c r="AP24" t="n">
-        <v>0.430712780954187</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
@@ -5153,15 +4928,6 @@
       </c>
       <c r="AM25" t="n">
         <v>0.450885898086805</v>
-      </c>
-      <c r="AN25" t="n">
-        <v>0.720088336791621</v>
-      </c>
-      <c r="AO25" t="n">
-        <v>0.738579994967044</v>
-      </c>
-      <c r="AP25" t="n">
-        <v>0.952012777369674</v>
       </c>
     </row>
   </sheetData>
@@ -5296,15 +5062,6 @@
       <c r="AM1" t="s">
         <v>277</v>
       </c>
-      <c r="AN1" t="s">
-        <v>278</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>279</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>280</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -5424,15 +5181,6 @@
       <c r="AM2" t="n">
         <v>0.263230303201223</v>
       </c>
-      <c r="AN2" t="n">
-        <v>0.413387626727509</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>0.230047498307442</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>0.122341422050048</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -5552,15 +5300,6 @@
       <c r="AM3" t="n">
         <v>0.153869376301927</v>
       </c>
-      <c r="AN3" t="n">
-        <v>0.428186865746061</v>
-      </c>
-      <c r="AO3" t="n">
-        <v>0.253411428865701</v>
-      </c>
-      <c r="AP3" t="n">
-        <v>0.213641068813313</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -5680,15 +5419,6 @@
       <c r="AM4" t="n">
         <v>0.665809427808503</v>
       </c>
-      <c r="AN4" t="n">
-        <v>0.987588742858819</v>
-      </c>
-      <c r="AO4" t="n">
-        <v>0.756918061292538</v>
-      </c>
-      <c r="AP4" t="n">
-        <v>0.810319629505895</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -5808,15 +5538,6 @@
       <c r="AM5" t="n">
         <v>-3.42464009737254</v>
       </c>
-      <c r="AN5" t="n">
-        <v>-3.39940055405</v>
-      </c>
-      <c r="AO5" t="n">
-        <v>-3.4947337506017</v>
-      </c>
-      <c r="AP5" t="n">
-        <v>-3.2856518195182</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -5936,15 +5657,6 @@
       <c r="AM6" t="n">
         <v>0.595432590846561</v>
       </c>
-      <c r="AN6" t="n">
-        <v>0.463270577579243</v>
-      </c>
-      <c r="AO6" t="n">
-        <v>0.365339489339483</v>
-      </c>
-      <c r="AP6" t="n">
-        <v>0.329230260915579</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -6064,15 +5776,6 @@
       <c r="AM7" t="n">
         <v>0.667649722621047</v>
       </c>
-      <c r="AN7" t="n">
-        <v>1.12899305989526</v>
-      </c>
-      <c r="AO7" t="n">
-        <v>0.560191901814442</v>
-      </c>
-      <c r="AP7" t="n">
-        <v>0.838479780897082</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -6192,15 +5895,6 @@
       <c r="AM8" t="n">
         <v>-0.0705474489869138</v>
       </c>
-      <c r="AN8" t="n">
-        <v>-0.143488438138486</v>
-      </c>
-      <c r="AO8" t="n">
-        <v>0.175109359749559</v>
-      </c>
-      <c r="AP8" t="n">
-        <v>0.259525600607175</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -6320,15 +6014,6 @@
       <c r="AM9" t="n">
         <v>0.376515468677237</v>
       </c>
-      <c r="AN9" t="n">
-        <v>0.440093363621778</v>
-      </c>
-      <c r="AO9" t="n">
-        <v>0.418062409358431</v>
-      </c>
-      <c r="AP9" t="n">
-        <v>0.416972281161938</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -6448,15 +6133,6 @@
       <c r="AM10" t="n">
         <v>0.324539836178846</v>
       </c>
-      <c r="AN10" t="n">
-        <v>0.354409543587638</v>
-      </c>
-      <c r="AO10" t="n">
-        <v>0.476448402857847</v>
-      </c>
-      <c r="AP10" t="n">
-        <v>0.434326926549304</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -6576,15 +6252,6 @@
       <c r="AM11" t="n">
         <v>0.535547041180719</v>
       </c>
-      <c r="AN11" t="n">
-        <v>0.578880457447692</v>
-      </c>
-      <c r="AO11" t="n">
-        <v>0.499770134961523</v>
-      </c>
-      <c r="AP11" t="n">
-        <v>0.507315066533857</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -6704,15 +6371,6 @@
       <c r="AM12" t="n">
         <v>0.406207073412492</v>
       </c>
-      <c r="AN12" t="n">
-        <v>0.519703250957127</v>
-      </c>
-      <c r="AO12" t="n">
-        <v>0.376455002322061</v>
-      </c>
-      <c r="AP12" t="n">
-        <v>0.392807811997798</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -6832,15 +6490,6 @@
       <c r="AM13" t="n">
         <v>0.355989261606786</v>
       </c>
-      <c r="AN13" t="n">
-        <v>0.471734051545736</v>
-      </c>
-      <c r="AO13" t="n">
-        <v>0.501710969402215</v>
-      </c>
-      <c r="AP13" t="n">
-        <v>0.580083403017813</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -6960,15 +6609,6 @@
       <c r="AM14" t="n">
         <v>-1.27447414535202</v>
       </c>
-      <c r="AN14" t="n">
-        <v>-1.28867082553521</v>
-      </c>
-      <c r="AO14" t="n">
-        <v>-0.88827469804023</v>
-      </c>
-      <c r="AP14" t="n">
-        <v>-0.948318550492076</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -7088,15 +6728,6 @@
       <c r="AM15" t="n">
         <v>-0.223546525250862</v>
       </c>
-      <c r="AN15" t="n">
-        <v>-0.428289481945481</v>
-      </c>
-      <c r="AO15" t="n">
-        <v>-0.137332879471191</v>
-      </c>
-      <c r="AP15" t="n">
-        <v>-0.108871346271135</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -7216,15 +6847,6 @@
       <c r="AM16" t="n">
         <v>-0.00259513083178143</v>
       </c>
-      <c r="AN16" t="n">
-        <v>0.232422845330032</v>
-      </c>
-      <c r="AO16" t="n">
-        <v>0.462568110113179</v>
-      </c>
-      <c r="AP16" t="n">
-        <v>0.504881523977443</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
@@ -7344,15 +6966,6 @@
       <c r="AM17" t="n">
         <v>1.72778649746387</v>
       </c>
-      <c r="AN17" t="n">
-        <v>1.00448805227021</v>
-      </c>
-      <c r="AO17" t="n">
-        <v>1.46144691989213</v>
-      </c>
-      <c r="AP17" t="n">
-        <v>0.987487759212215</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -7472,15 +7085,6 @@
       <c r="AM18" t="n">
         <v>0.47460609290998</v>
       </c>
-      <c r="AN18" t="n">
-        <v>0.0432909745533368</v>
-      </c>
-      <c r="AO18" t="n">
-        <v>0.305383771525753</v>
-      </c>
-      <c r="AP18" t="n">
-        <v>0.478522679470589</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -7600,15 +7204,6 @@
       <c r="AM19" t="n">
         <v>-0.617194144022358</v>
       </c>
-      <c r="AN19" t="n">
-        <v>-0.441485112092623</v>
-      </c>
-      <c r="AO19" t="n">
-        <v>-0.215952056008671</v>
-      </c>
-      <c r="AP19" t="n">
-        <v>-0.425345030924153</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -7728,15 +7323,6 @@
       <c r="AM20" t="n">
         <v>-0.0127085434799633</v>
       </c>
-      <c r="AN20" t="n">
-        <v>-0.912815189455095</v>
-      </c>
-      <c r="AO20" t="n">
-        <v>-0.929794630762767</v>
-      </c>
-      <c r="AP20" t="n">
-        <v>-0.695806559425522</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -7856,15 +7442,6 @@
       <c r="AM21" t="n">
         <v>-0.909778505929621</v>
       </c>
-      <c r="AN21" t="n">
-        <v>-1.05113704457584</v>
-      </c>
-      <c r="AO21" t="n">
-        <v>-1.54651252586074</v>
-      </c>
-      <c r="AP21" t="n">
-        <v>-1.99467874840897</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
@@ -7984,15 +7561,6 @@
       <c r="AM22" t="n">
         <v>-1.49268743353787</v>
       </c>
-      <c r="AN22" t="n">
-        <v>-1.14992629800796</v>
-      </c>
-      <c r="AO22" t="n">
-        <v>-1.09692410616963</v>
-      </c>
-      <c r="AP22" t="n">
-        <v>-1.13210673842294</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -8112,15 +7680,6 @@
       <c r="AM23" t="n">
         <v>0.358292119639118</v>
       </c>
-      <c r="AN23" t="n">
-        <v>0.363187223794476</v>
-      </c>
-      <c r="AO23" t="n">
-        <v>0.308171412091469</v>
-      </c>
-      <c r="AP23" t="n">
-        <v>0.332118020429082</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
@@ -8240,15 +7799,6 @@
       <c r="AM24" t="n">
         <v>0.671811264828821</v>
       </c>
-      <c r="AN24" t="n">
-        <v>0.665487971094159</v>
-      </c>
-      <c r="AO24" t="n">
-        <v>0.419909780054107</v>
-      </c>
-      <c r="AP24" t="n">
-        <v>0.430712780954187</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
@@ -8367,15 +7917,6 @@
       </c>
       <c r="AM25" t="n">
         <v>0.450885898086805</v>
-      </c>
-      <c r="AN25" t="n">
-        <v>0.720088336791621</v>
-      </c>
-      <c r="AO25" t="n">
-        <v>0.738579994967044</v>
-      </c>
-      <c r="AP25" t="n">
-        <v>0.952012777369674</v>
       </c>
     </row>
   </sheetData>

</xml_diff>